<commit_message>
Fixed tags and parsing new pozzi
to test
</commit_message>
<xml_diff>
--- a/Automatisms/pozzi_tags/Tag Pozzi con Sonde_per TLC_1.xlsx
+++ b/Automatisms/pozzi_tags/Tag Pozzi con Sonde_per TLC_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloferaudo/Desktop/Personal Data/Research activities/Unibo/Progetto_HERA_ARPAE/Automatisms/pozzi_tags/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A97537-073A-584C-87A4-26A67720DF96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E48B8B-3F2D-D445-AFBF-630989F49933}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="760" windowWidth="21480" windowHeight="13140" xr2:uid="{4B4D8BA3-11DD-45BD-9E66-A95A3732EAEC}"/>
   </bookViews>
@@ -187,21 +187,12 @@
     <t>B012719ABO13_1_J_LIV_FALD008_MFLIV01</t>
   </si>
   <si>
-    <t>B012719ABO13_1_J_SIN_PMSL008_SFONN01</t>
-  </si>
-  <si>
     <t>B012935ABO13_1_J_LIV_FALD001_MFLIV01</t>
   </si>
   <si>
-    <t>B012935ABO13_1_J_SIN_PMSL001_SFONN01</t>
-  </si>
-  <si>
     <t>B017237ABO19_1_J_LIV_FALD007_MFLIV03</t>
   </si>
   <si>
-    <t>B017237ABO19_1_J_SIN_PMSL005_SFONN01</t>
-  </si>
-  <si>
     <t>BoPan8</t>
   </si>
   <si>
@@ -224,6 +215,15 @@
   </si>
   <si>
     <t>TYPE</t>
+  </si>
+  <si>
+    <t>B017237ABO19_1_J_SIN_PMSL005_MFASS01</t>
+  </si>
+  <si>
+    <t>B012935ABO13_1_J_SIN_PMSL001_MFASS01</t>
+  </si>
+  <si>
+    <t>B012719ABO13_1_J_SIN_PMSL008_MFASS01</t>
   </si>
 </sst>
 </file>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED342DA-4F64-4966-8F46-0D3D9D7E0BD7}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -700,10 +700,10 @@
         <v>32</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1000,19 +1000,19 @@
         <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1">
         <v>70</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1026,19 +1026,19 @@
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1">
         <v>70</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1052,19 +1052,19 @@
         <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F15" s="1">
         <v>70</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1072,16 +1072,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F16">
         <v>8.8000000000000007</v>

</xml_diff>